<commit_message>
Atualização dos entregáveis de engenharia de software
Foram disponibilizados na pasta EngenhariaDeSoftware os últimos documentos de controle do projeto
</commit_message>
<xml_diff>
--- a/EngenhariaDeSoftware/Avas/AVA.xlsx
+++ b/EngenhariaDeSoftware/Avas/AVA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Esforço plannejado</t>
   </si>
@@ -117,16 +117,37 @@
     <t>SPI</t>
   </si>
   <si>
+    <t>P IA</t>
+  </si>
+  <si>
     <t>SV</t>
   </si>
   <si>
+    <t>BD</t>
+  </si>
+  <si>
     <t>CPI</t>
   </si>
   <si>
+    <t>LFG</t>
+  </si>
+  <si>
     <t>CV</t>
   </si>
   <si>
+    <t>VE</t>
+  </si>
+  <si>
     <t>Homens hora esforço real</t>
+  </si>
+  <si>
+    <t>bf</t>
+  </si>
+  <si>
+    <t>ct</t>
+  </si>
+  <si>
+    <t>mv</t>
   </si>
   <si>
     <t>PV</t>
@@ -307,11 +328,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1921809907"/>
-        <c:axId val="26775557"/>
+        <c:axId val="1983578318"/>
+        <c:axId val="950050439"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1921809907"/>
+        <c:axId val="1983578318"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -363,10 +384,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26775557"/>
+        <c:crossAx val="950050439"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26775557"/>
+        <c:axId val="950050439"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,7 +451,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1921809907"/>
+        <c:crossAx val="1983578318"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -494,7 +515,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$E$26:$L$26</c:f>
+              <c:f>Planilha1!$E$26:$P$26</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
@@ -523,17 +544,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$E$27:$L$27</c:f>
+              <c:f>Planilha1!$E$27:$P$27</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1850799508"/>
-        <c:axId val="336319335"/>
+        <c:axId val="64893874"/>
+        <c:axId val="1760303371"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1850799508"/>
+        <c:axId val="64893874"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,10 +606,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="336319335"/>
+        <c:crossAx val="1760303371"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="336319335"/>
+        <c:axId val="1760303371"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,7 +673,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1850799508"/>
+        <c:crossAx val="64893874"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1223,19 +1244,19 @@
       </c>
       <c r="M10" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5225.21449</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5284.795043</v>
       </c>
       <c r="O10" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5284.795043</v>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6250</v>
       </c>
     </row>
     <row r="11">
@@ -1276,19 +1297,19 @@
       </c>
       <c r="M11" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>83.60343184</v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>84.55672069</v>
       </c>
       <c r="O11" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>84.55672069</v>
       </c>
       <c r="P11" s="1">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12">
@@ -1319,10 +1340,18 @@
       <c r="L12" s="5">
         <v>87.1</v>
       </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="M12" s="5">
+        <v>87.7</v>
+      </c>
+      <c r="N12" s="5">
+        <v>88.7</v>
+      </c>
+      <c r="O12" s="5">
+        <v>88.7</v>
+      </c>
+      <c r="P12" s="5">
+        <v>104.9</v>
+      </c>
     </row>
     <row r="13">
       <c r="D13" s="4" t="s">
@@ -1362,19 +1391,19 @@
       </c>
       <c r="M13" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5106.053384</v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5195.424214</v>
       </c>
       <c r="O13" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5195.424214</v>
       </c>
       <c r="P13" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>6446.615825</v>
       </c>
     </row>
     <row r="14">
@@ -1415,25 +1444,31 @@
       </c>
       <c r="M14" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.9379679144</v>
       </c>
       <c r="N14" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.9317226891</v>
       </c>
       <c r="O14" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.8790882061</v>
       </c>
       <c r="P14" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S14" s="2">
+        <v>360.0</v>
       </c>
       <c r="T14" s="2"/>
     </row>
     <row r="15">
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" ref="E15:P15" si="8">E10-E8</f>
@@ -1469,25 +1504,31 @@
       </c>
       <c r="M15" s="1">
         <f t="shared" si="8"/>
-        <v>-5570.781697</v>
+        <v>-345.5672069</v>
       </c>
       <c r="N15" s="1">
         <f t="shared" si="8"/>
-        <v>-5672.068637</v>
+        <v>-387.2735939</v>
       </c>
       <c r="O15" s="1">
         <f t="shared" si="8"/>
-        <v>-6011.677788</v>
+        <v>-726.8827455</v>
       </c>
       <c r="P15" s="1">
         <f t="shared" si="8"/>
-        <v>-6250</v>
-      </c>
-      <c r="T15" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S15" s="2">
+        <v>345.0</v>
+      </c>
+      <c r="W15" s="2"/>
     </row>
     <row r="16">
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" ref="E16:P16" si="9">E10/E13</f>
@@ -1521,27 +1562,33 @@
         <f t="shared" si="9"/>
         <v>1.06936771</v>
       </c>
-      <c r="M16" s="1" t="str">
+      <c r="M16" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" s="1" t="str">
+        <v>1.023337223</v>
+      </c>
+      <c r="N16" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="1" t="str">
+        <v>1.017201835</v>
+      </c>
+      <c r="O16" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P16" s="1" t="str">
+        <v>1.017201835</v>
+      </c>
+      <c r="P16" s="1">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0.9695009242</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S16" s="2">
+        <v>30.0</v>
       </c>
       <c r="T16" s="2"/>
     </row>
     <row r="17">
       <c r="D17" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" ref="E17:P17" si="10">E10-E13</f>
@@ -1577,24 +1624,30 @@
       </c>
       <c r="M17" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>119.1611058</v>
       </c>
       <c r="N17" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>89.37082936</v>
       </c>
       <c r="O17" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>89.37082936</v>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-196.6158246</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S17" s="2">
+        <v>180.0</v>
       </c>
     </row>
     <row r="18">
       <c r="D18" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E18" s="3">
         <v>1.75</v>
@@ -1620,21 +1673,52 @@
       <c r="L18" s="5">
         <v>81.45</v>
       </c>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
+      <c r="M18" s="5">
+        <v>85.7</v>
+      </c>
+      <c r="N18" s="5">
+        <v>87.2</v>
+      </c>
+      <c r="O18" s="5">
+        <v>87.2</v>
+      </c>
+      <c r="P18" s="5">
+        <v>108.2</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S18" s="2">
+        <v>90.0</v>
+      </c>
     </row>
     <row r="19">
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="R19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S19" s="2">
+        <v>240.0</v>
+      </c>
       <c r="T19" s="5"/>
     </row>
     <row r="20">
-      <c r="T20" s="2"/>
+      <c r="R20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S20" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="T20" s="2">
+        <f>SUM(S14:S20)/60</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
       <c r="D22" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E22" s="1">
         <v>104.26596758817921</v>
@@ -1675,7 +1759,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E23" s="1">
         <v>104.26596758817921</v>
@@ -1700,11 +1784,23 @@
       </c>
       <c r="L23" s="6">
         <v>5189.466158245948</v>
+      </c>
+      <c r="M23" s="6">
+        <v>5225.214489990467</v>
+      </c>
+      <c r="N23" s="6">
+        <v>5284.795042897998</v>
+      </c>
+      <c r="O23" s="6">
+        <v>5284.795042897998</v>
+      </c>
+      <c r="P23" s="6">
+        <v>6250.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E24" s="1">
         <v>104.26596758817921</v>
@@ -1729,6 +1825,18 @@
       </c>
       <c r="L24" s="6">
         <v>4852.836034318399</v>
+      </c>
+      <c r="M24" s="6">
+        <v>5106.053384175405</v>
+      </c>
+      <c r="N24" s="6">
+        <v>5195.424213536701</v>
+      </c>
+      <c r="O24" s="6">
+        <v>5195.424213536701</v>
+      </c>
+      <c r="P24" s="1">
+        <v>6446.615824594852</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
@@ -1737,73 +1845,81 @@
         <v>32</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ref="E26:L26" si="11">E23/E22</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="11"/>
-        <v>1.032679739</v>
+        <v>1.0326797385620916</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="11"/>
-        <v>0.9940079893</v>
+        <v>0.9940079893475369</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="11"/>
-        <v>0.950062422</v>
+        <v>0.9500624219725345</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="11"/>
-        <v>0.9879663057</v>
+        <v>0.9879663056558362</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="11"/>
-        <v>0.990815155</v>
+        <v>0.9908151549942597</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="11"/>
-        <v>0.9560922064</v>
+        <v>0.9560922063666301</v>
+      </c>
+      <c r="M26" s="6">
+        <v>0.9379679144385027</v>
+      </c>
+      <c r="N26" s="6">
+        <v>0.9317226890756304</v>
+      </c>
+      <c r="O26" s="6">
+        <v>0.8790882061446976</v>
+      </c>
+      <c r="P26" s="6">
+        <v>1.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="D27" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" ref="E27:L27" si="12">E23/E24</f>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="12"/>
-        <v>1.277159966</v>
+        <v>1.2771599657827204</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="12"/>
-        <v>1.21857486</v>
+        <v>1.2185748598879103</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="12"/>
-        <v>1.110209601</v>
+        <v>1.1102096010818119</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="12"/>
-        <v>1.086217747</v>
+        <v>1.0862177470106984</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="12"/>
-        <v>1.06936771</v>
+        <v>1.0693677102516879</v>
+      </c>
+      <c r="M27" s="6">
+        <v>1.0233372228704785</v>
+      </c>
+      <c r="N27" s="6">
+        <v>1.0172018348623855</v>
+      </c>
+      <c r="O27" s="6">
+        <v>1.0172018348623855</v>
+      </c>
+      <c r="P27" s="6">
+        <v>0.9695009242144178</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1"/>

</xml_diff>